<commit_message>
[Pipette] Transformer 부품 검토 - 가격 및 agency
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Review Data_20180203.xlsx
+++ b/Plasma_Gen_Review Data_20180203.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="시제품_Pulse" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pin-map'!$B$15:$AB$79</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="602">
   <si>
     <t>각 mode 별 Pulse 출력</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2347,107 +2347,115 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ICbanQ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레오콤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTX210611</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>품절</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOSFET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRFS4410PbF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">INFINEON </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET, N-CH, 100V, 97A, TO-263 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTD5802N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semiconductor </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power MOSFET 40V, Single N−Channel, 101A DPAK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTX210605-R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COOPER BUSSMANN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 4W 10V 7MA SMD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W 15V 11MA SMD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W 20V 11MA SMD Turn-R:67</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W 15V 11MA SMD Turn-R:86</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W 11V 11MA SMD Turn-R:125</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DVM 측정치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OFF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>CTX210611-R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICbanQ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레오콤</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTX210611</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>재고</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>품절</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOSFET</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRFS4410PbF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">INFINEON </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET, N-CH, 100V, 97A, TO-263 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NTD5802N</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ON Semiconductor </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power MOSFET 40V, Single N−Channel, 101A DPAK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTX210605-R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COOPER BUSSMANN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 4W 10V 7MA SMD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W 15V 11MA SMD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W 20V 11MA SMD Turn-R:67</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W 15V 11MA SMD Turn-R:86</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W 11V 11MA SMD Turn-R:125</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DVM 측정치</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OFF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ON</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plasma On</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2610,7 +2618,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2918,6 +2926,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2926,7 +2945,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3401,120 +3420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3527,6 +3432,126 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
@@ -5209,7 +5234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5244,7 +5269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5519,22 +5544,22 @@
       <c r="E123" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F123" s="188" t="s">
+      <c r="F123" s="198" t="s">
         <v>11</v>
       </c>
-      <c r="G123" s="196"/>
-      <c r="H123" s="188" t="s">
+      <c r="G123" s="206"/>
+      <c r="H123" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="I123" s="196"/>
-      <c r="J123" s="188" t="s">
+      <c r="I123" s="206"/>
+      <c r="J123" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="K123" s="189"/>
-      <c r="L123" s="188" t="s">
+      <c r="K123" s="199"/>
+      <c r="L123" s="198" t="s">
         <v>547</v>
       </c>
-      <c r="M123" s="189"/>
+      <c r="M123" s="199"/>
     </row>
     <row r="124" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D124" s="4" t="s">
@@ -5543,20 +5568,20 @@
       <c r="E124" s="5">
         <v>80</v>
       </c>
-      <c r="F124" s="190">
+      <c r="F124" s="200">
         <v>829.5</v>
       </c>
-      <c r="G124" s="190"/>
-      <c r="H124" s="190">
+      <c r="G124" s="200"/>
+      <c r="H124" s="200">
         <v>20</v>
       </c>
-      <c r="I124" s="190"/>
-      <c r="J124" s="190">
+      <c r="I124" s="200"/>
+      <c r="J124" s="200">
         <v>40</v>
       </c>
-      <c r="K124" s="190"/>
-      <c r="L124" s="190"/>
-      <c r="M124" s="191"/>
+      <c r="K124" s="200"/>
+      <c r="L124" s="200"/>
+      <c r="M124" s="201"/>
     </row>
     <row r="125" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D125" s="6" t="s">
@@ -5565,20 +5590,20 @@
       <c r="E125" s="7">
         <v>80</v>
       </c>
-      <c r="F125" s="192">
+      <c r="F125" s="202">
         <v>829.5</v>
       </c>
-      <c r="G125" s="192"/>
-      <c r="H125" s="192">
+      <c r="G125" s="202"/>
+      <c r="H125" s="202">
         <v>10</v>
       </c>
-      <c r="I125" s="192"/>
-      <c r="J125" s="192">
+      <c r="I125" s="202"/>
+      <c r="J125" s="202">
         <v>20</v>
       </c>
-      <c r="K125" s="192"/>
-      <c r="L125" s="192"/>
-      <c r="M125" s="193"/>
+      <c r="K125" s="202"/>
+      <c r="L125" s="202"/>
+      <c r="M125" s="203"/>
     </row>
     <row r="126" spans="3:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D126" s="8" t="s">
@@ -5587,18 +5612,18 @@
       <c r="E126" s="9">
         <v>80</v>
       </c>
-      <c r="F126" s="194">
+      <c r="F126" s="204">
         <v>829.5</v>
       </c>
-      <c r="G126" s="194"/>
-      <c r="H126" s="194">
+      <c r="G126" s="204"/>
+      <c r="H126" s="204">
         <v>10</v>
       </c>
-      <c r="I126" s="194"/>
-      <c r="J126" s="194"/>
-      <c r="K126" s="194"/>
-      <c r="L126" s="194"/>
-      <c r="M126" s="195"/>
+      <c r="I126" s="204"/>
+      <c r="J126" s="204"/>
+      <c r="K126" s="204"/>
+      <c r="L126" s="204"/>
+      <c r="M126" s="205"/>
     </row>
     <row r="128" spans="3:13" x14ac:dyDescent="0.3">
       <c r="E128">
@@ -6090,10 +6115,10 @@
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="212" t="s">
+      <c r="B3" s="222" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="213"/>
+      <c r="C3" s="223"/>
       <c r="D3" s="13">
         <v>128</v>
       </c>
@@ -6112,10 +6137,10 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="214" t="s">
+      <c r="B4" s="224" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="215"/>
+      <c r="C4" s="225"/>
       <c r="D4" s="16">
         <v>16</v>
       </c>
@@ -6135,10 +6160,10 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="214" t="s">
+      <c r="B5" s="224" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="215"/>
+      <c r="C5" s="225"/>
       <c r="D5" s="16">
         <v>48</v>
       </c>
@@ -6160,10 +6185,10 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="214" t="s">
+      <c r="B6" s="224" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="215"/>
+      <c r="C6" s="225"/>
       <c r="D6" s="16" t="s">
         <v>34</v>
       </c>
@@ -6180,10 +6205,10 @@
       <c r="Q6" s="67"/>
     </row>
     <row r="7" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="226" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="217"/>
+      <c r="C7" s="227"/>
       <c r="D7" s="19" t="s">
         <v>37</v>
       </c>
@@ -6252,39 +6277,39 @@
     </row>
     <row r="13" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="208" t="s">
+      <c r="B14" s="218" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="202"/>
-      <c r="D14" s="202" t="s">
+      <c r="C14" s="212"/>
+      <c r="D14" s="212" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="202" t="s">
+      <c r="E14" s="212" t="s">
         <v>236</v>
       </c>
-      <c r="F14" s="203"/>
-      <c r="G14" s="209" t="s">
+      <c r="F14" s="213"/>
+      <c r="G14" s="219" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="210"/>
-      <c r="I14" s="209" t="s">
+      <c r="H14" s="220"/>
+      <c r="I14" s="219" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="210"/>
-      <c r="K14" s="209" t="s">
+      <c r="J14" s="220"/>
+      <c r="K14" s="219" t="s">
         <v>224</v>
       </c>
-      <c r="L14" s="201"/>
+      <c r="L14" s="211"/>
       <c r="M14" s="78"/>
       <c r="N14" s="96"/>
-      <c r="O14" s="209" t="s">
+      <c r="O14" s="219" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="201"/>
-      <c r="Q14" s="201" t="s">
+      <c r="P14" s="211"/>
+      <c r="Q14" s="211" t="s">
         <v>225</v>
       </c>
-      <c r="R14" s="201"/>
+      <c r="R14" s="211"/>
       <c r="S14" s="129"/>
       <c r="T14" s="94"/>
     </row>
@@ -6295,7 +6320,7 @@
       <c r="C15" s="64" t="s">
         <v>251</v>
       </c>
-      <c r="D15" s="211"/>
+      <c r="D15" s="221"/>
       <c r="E15" s="64" t="s">
         <v>320</v>
       </c>
@@ -6355,10 +6380,10 @@
       <c r="D16" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="204" t="s">
+      <c r="E16" s="214" t="s">
         <v>247</v>
       </c>
-      <c r="F16" s="205"/>
+      <c r="F16" s="215"/>
       <c r="G16" s="111"/>
       <c r="H16" s="144"/>
       <c r="I16" s="154"/>
@@ -6605,10 +6630,10 @@
       <c r="D22" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="206" t="s">
+      <c r="E22" s="216" t="s">
         <v>248</v>
       </c>
-      <c r="F22" s="207"/>
+      <c r="F22" s="217"/>
       <c r="G22" s="139"/>
       <c r="H22" s="98"/>
       <c r="I22" s="84"/>
@@ -6852,10 +6877,10 @@
       <c r="D27" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="E27" s="197" t="s">
+      <c r="E27" s="207" t="s">
         <v>260</v>
       </c>
-      <c r="F27" s="198"/>
+      <c r="F27" s="208"/>
       <c r="G27" s="140"/>
       <c r="H27" s="100"/>
       <c r="I27" s="84"/>
@@ -6881,10 +6906,10 @@
       <c r="D28" s="82" t="s">
         <v>259</v>
       </c>
-      <c r="E28" s="197" t="s">
+      <c r="E28" s="207" t="s">
         <v>261</v>
       </c>
-      <c r="F28" s="198"/>
+      <c r="F28" s="208"/>
       <c r="G28" s="140"/>
       <c r="H28" s="100"/>
       <c r="I28" s="84"/>
@@ -7082,10 +7107,10 @@
       <c r="D33" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E33" s="197" t="s">
+      <c r="E33" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F33" s="198"/>
+      <c r="F33" s="208"/>
       <c r="G33" s="140"/>
       <c r="H33" s="100"/>
       <c r="I33" s="84"/>
@@ -7111,10 +7136,10 @@
       <c r="D34" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E34" s="197" t="s">
+      <c r="E34" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="F34" s="198"/>
+      <c r="F34" s="208"/>
       <c r="G34" s="140"/>
       <c r="H34" s="100"/>
       <c r="I34" s="84"/>
@@ -7744,10 +7769,10 @@
       <c r="D46" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E46" s="197" t="s">
+      <c r="E46" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F46" s="198"/>
+      <c r="F46" s="208"/>
       <c r="G46" s="140"/>
       <c r="H46" s="100"/>
       <c r="I46" s="84"/>
@@ -7773,10 +7798,10 @@
       <c r="D47" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="197" t="s">
+      <c r="E47" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="F47" s="198"/>
+      <c r="F47" s="208"/>
       <c r="G47" s="140"/>
       <c r="H47" s="100"/>
       <c r="I47" s="84"/>
@@ -8517,10 +8542,10 @@
       <c r="D62" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E62" s="197" t="s">
+      <c r="E62" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F62" s="198"/>
+      <c r="F62" s="208"/>
       <c r="G62" s="140"/>
       <c r="H62" s="100"/>
       <c r="I62" s="84"/>
@@ -8546,10 +8571,10 @@
       <c r="D63" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E63" s="197" t="s">
+      <c r="E63" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="F63" s="198"/>
+      <c r="F63" s="208"/>
       <c r="G63" s="140"/>
       <c r="H63" s="100"/>
       <c r="I63" s="84"/>
@@ -9160,10 +9185,10 @@
       <c r="D75" s="109" t="s">
         <v>297</v>
       </c>
-      <c r="E75" s="197" t="s">
+      <c r="E75" s="207" t="s">
         <v>316</v>
       </c>
-      <c r="F75" s="198"/>
+      <c r="F75" s="208"/>
       <c r="G75" s="140"/>
       <c r="H75" s="136"/>
       <c r="I75" s="85"/>
@@ -9311,10 +9336,10 @@
       <c r="D78" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E78" s="197" t="s">
+      <c r="E78" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F78" s="198"/>
+      <c r="F78" s="208"/>
       <c r="G78" s="140"/>
       <c r="H78" s="100"/>
       <c r="I78" s="84"/>
@@ -9340,10 +9365,10 @@
       <c r="D79" s="88" t="s">
         <v>235</v>
       </c>
-      <c r="E79" s="199" t="s">
+      <c r="E79" s="209" t="s">
         <v>247</v>
       </c>
-      <c r="F79" s="200"/>
+      <c r="F79" s="210"/>
       <c r="G79" s="141"/>
       <c r="H79" s="143"/>
       <c r="I79" s="148"/>
@@ -9445,11 +9470,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J37"/>
+  <dimension ref="B1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9500,7 +9525,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="221" t="s">
+      <c r="B4" s="233" t="s">
         <v>332</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -9525,7 +9550,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="218"/>
+      <c r="B5" s="230"/>
       <c r="C5" s="7" t="s">
         <v>211</v>
       </c>
@@ -9545,7 +9570,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="218"/>
+      <c r="B6" s="230"/>
       <c r="C6" s="7" t="s">
         <v>218</v>
       </c>
@@ -9565,7 +9590,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="218" t="s">
+      <c r="B7" s="230" t="s">
         <v>217</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -9587,7 +9612,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="218"/>
+      <c r="B8" s="230"/>
       <c r="C8" s="7" t="s">
         <v>219</v>
       </c>
@@ -9607,7 +9632,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="218" t="s">
+      <c r="B9" s="230" t="s">
         <v>226</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -9627,7 +9652,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="219"/>
+      <c r="B10" s="231"/>
       <c r="C10" s="9" t="s">
         <v>231</v>
       </c>
@@ -9647,7 +9672,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="220" t="s">
+      <c r="B11" s="232" t="s">
         <v>401</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -9669,7 +9694,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="218"/>
+      <c r="B12" s="230"/>
       <c r="C12" s="39" t="s">
         <v>329</v>
       </c>
@@ -9689,7 +9714,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="219"/>
+      <c r="B13" s="231"/>
       <c r="C13" s="45" t="s">
         <v>364</v>
       </c>
@@ -9709,7 +9734,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="220" t="s">
+      <c r="B14" s="232" t="s">
         <v>333</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -9731,7 +9756,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="219"/>
+      <c r="B15" s="231"/>
       <c r="C15" s="45" t="s">
         <v>415</v>
       </c>
@@ -9751,7 +9776,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="224" t="s">
+      <c r="B16" s="236" t="s">
         <v>416</v>
       </c>
       <c r="C16" s="44" t="s">
@@ -9773,7 +9798,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="225"/>
+      <c r="B17" s="237"/>
       <c r="C17" s="119" t="s">
         <v>513</v>
       </c>
@@ -9795,7 +9820,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="225"/>
+      <c r="B18" s="237"/>
       <c r="C18" s="118" t="s">
         <v>522</v>
       </c>
@@ -9815,7 +9840,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="223"/>
+      <c r="B19" s="235"/>
       <c r="C19" s="118" t="s">
         <v>524</v>
       </c>
@@ -9835,7 +9860,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="222" t="s">
+      <c r="B20" s="234" t="s">
         <v>422</v>
       </c>
       <c r="C20" s="39" t="s">
@@ -9857,7 +9882,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="223"/>
+      <c r="B21" s="235"/>
       <c r="C21" s="118" t="s">
         <v>519</v>
       </c>
@@ -9877,7 +9902,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="218" t="s">
+      <c r="B22" s="230" t="s">
         <v>436</v>
       </c>
       <c r="C22" s="39" t="s">
@@ -9899,7 +9924,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="218"/>
+      <c r="B23" s="230"/>
       <c r="C23" s="39" t="s">
         <v>452</v>
       </c>
@@ -10006,7 +10031,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="218" t="s">
+      <c r="B28" s="230" t="s">
         <v>486</v>
       </c>
       <c r="C28" s="39" t="s">
@@ -10031,7 +10056,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="218"/>
+      <c r="B29" s="230"/>
       <c r="C29" s="39" t="s">
         <v>484</v>
       </c>
@@ -10054,7 +10079,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="219"/>
+      <c r="B30" s="231"/>
       <c r="C30" s="45" t="s">
         <v>485</v>
       </c>
@@ -10101,65 +10126,68 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="10" t="s">
-        <v>552</v>
-      </c>
-      <c r="C32" s="226" t="s">
+      <c r="B32" s="229" t="s">
+        <v>599</v>
+      </c>
+      <c r="C32" s="188" t="s">
         <v>559</v>
       </c>
       <c r="D32" t="s">
         <v>551</v>
       </c>
-      <c r="E32" s="226" t="s">
+      <c r="E32" s="188" t="s">
         <v>553</v>
       </c>
       <c r="H32" s="41"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C33" s="226" t="s">
+      <c r="B33" s="228"/>
+      <c r="C33" s="188" t="s">
         <v>560</v>
       </c>
       <c r="D33" t="s">
         <v>551</v>
       </c>
-      <c r="E33" s="226" t="s">
+      <c r="E33" s="188" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C34" s="226" t="s">
+      <c r="B34" s="228"/>
+      <c r="C34" s="188" t="s">
         <v>555</v>
       </c>
       <c r="D34" t="s">
         <v>551</v>
       </c>
-      <c r="E34" s="226" t="s">
+      <c r="E34" s="188" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C35" s="226" t="s">
+      <c r="B35" s="228"/>
+      <c r="C35" s="188" t="s">
         <v>557</v>
       </c>
       <c r="D35" t="s">
         <v>551</v>
       </c>
-      <c r="E35" s="226" t="s">
+      <c r="E35" s="188" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="228" t="s">
+        <v>579</v>
+      </c>
+      <c r="C36" s="188" t="s">
         <v>580</v>
       </c>
-      <c r="C36" s="226" t="s">
+      <c r="D36" t="s">
         <v>581</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="188" t="s">
         <v>582</v>
-      </c>
-      <c r="E36" s="226" t="s">
-        <v>583</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -10172,37 +10200,45 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="230" t="s">
+      <c r="B37" s="228"/>
+      <c r="C37" s="192" t="s">
+        <v>583</v>
+      </c>
+      <c r="D37" s="193" t="s">
         <v>584</v>
       </c>
-      <c r="D37" s="231" t="s">
+      <c r="E37" s="192" t="s">
         <v>585</v>
       </c>
-      <c r="E37" s="230" t="s">
-        <v>586</v>
-      </c>
-      <c r="F37" s="231"/>
-      <c r="G37" s="231">
+      <c r="F37" s="193"/>
+      <c r="G37" s="193">
         <v>1</v>
       </c>
-      <c r="H37" s="232">
+      <c r="H37" s="194">
         <v>1450</v>
       </c>
-      <c r="I37" s="233" t="s">
+      <c r="I37" s="195" t="s">
         <v>213</v>
       </c>
     </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B14:B15"/>
+  <mergeCells count="11">
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10237,30 +10273,30 @@
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" s="21"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="190" t="s">
+      <c r="E2" s="200" t="s">
         <v>337</v>
       </c>
-      <c r="F2" s="190"/>
-      <c r="G2" s="190" t="s">
+      <c r="F2" s="200"/>
+      <c r="G2" s="200" t="s">
         <v>340</v>
       </c>
-      <c r="H2" s="190"/>
-      <c r="I2" s="190" t="s">
+      <c r="H2" s="200"/>
+      <c r="I2" s="200" t="s">
         <v>342</v>
       </c>
-      <c r="J2" s="190"/>
+      <c r="J2" s="200"/>
       <c r="K2" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="L2" s="190" t="s">
+      <c r="L2" s="200" t="s">
         <v>343</v>
       </c>
-      <c r="M2" s="190"/>
-      <c r="N2" s="190" t="s">
+      <c r="M2" s="200"/>
+      <c r="N2" s="200" t="s">
         <v>344</v>
       </c>
-      <c r="O2" s="190"/>
-      <c r="P2" s="190"/>
+      <c r="O2" s="200"/>
+      <c r="P2" s="200"/>
       <c r="Q2" s="5" t="s">
         <v>349</v>
       </c>
@@ -11099,7 +11135,7 @@
       </c>
     </row>
     <row r="148" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C148" s="221" t="s">
+      <c r="C148" s="233" t="s">
         <v>401</v>
       </c>
       <c r="D148" s="45" t="s">
@@ -11120,7 +11156,7 @@
       </c>
     </row>
     <row r="149" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C149" s="218"/>
+      <c r="C149" s="230"/>
       <c r="D149" s="7" t="s">
         <v>392</v>
       </c>
@@ -11139,7 +11175,7 @@
       </c>
     </row>
     <row r="150" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C150" s="218"/>
+      <c r="C150" s="230"/>
       <c r="D150" s="7" t="s">
         <v>402</v>
       </c>
@@ -11358,10 +11394,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:S15"/>
+  <dimension ref="B4:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11371,12 +11407,12 @@
     <col min="14" max="14" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C5" s="185" t="s">
         <v>542</v>
       </c>
@@ -11390,7 +11426,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C6" s="186" t="s">
         <v>498</v>
       </c>
@@ -11404,7 +11440,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="187" t="s">
         <v>546</v>
       </c>
@@ -11420,34 +11456,34 @@
         <v>545</v>
       </c>
       <c r="N7" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
         <v>596</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="N8" t="s">
-        <v>597</v>
       </c>
       <c r="O8">
         <v>0.31</v>
       </c>
       <c r="P8" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="O9">
         <v>18.16</v>
       </c>
       <c r="P9" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N10" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="Q10">
         <v>760</v>
@@ -11459,7 +11495,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N11">
         <v>1</v>
       </c>
@@ -11467,22 +11503,26 @@
         <v>320</v>
       </c>
       <c r="P11" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q11" s="235">
+        <v>594</v>
+      </c>
+      <c r="Q11" s="197">
         <f>Q$10/$O11</f>
         <v>2.375</v>
       </c>
-      <c r="R11" s="235">
+      <c r="R11" s="197">
         <f>R$10/$O11</f>
         <v>3.75</v>
       </c>
-      <c r="S11" s="235">
+      <c r="S11" s="197">
         <f>S$10/$O11</f>
         <v>4.6875</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="T11">
+        <f>O11*4</f>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N12">
         <v>2</v>
       </c>
@@ -11491,22 +11531,26 @@
         <v>640</v>
       </c>
       <c r="P12" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q12" s="235">
+        <v>594</v>
+      </c>
+      <c r="Q12" s="197">
         <f t="shared" ref="Q12:S15" si="0">Q$10/$O12</f>
         <v>1.1875</v>
       </c>
-      <c r="R12" s="235">
+      <c r="R12" s="197">
         <f t="shared" si="0"/>
         <v>1.875</v>
       </c>
-      <c r="S12" s="235">
+      <c r="S12" s="197">
         <f t="shared" si="0"/>
         <v>2.34375</v>
       </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="T12">
+        <f t="shared" ref="T12:T15" si="1">O12*4</f>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N13">
         <v>3</v>
       </c>
@@ -11515,22 +11559,26 @@
         <v>960</v>
       </c>
       <c r="P13" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q13" s="235">
+        <v>594</v>
+      </c>
+      <c r="Q13" s="197">
         <f t="shared" si="0"/>
         <v>0.79166666666666663</v>
       </c>
-      <c r="R13" s="235">
+      <c r="R13" s="197">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="S13" s="235">
+      <c r="S13" s="197">
         <f t="shared" si="0"/>
         <v>1.5625</v>
       </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N14">
         <v>4</v>
       </c>
@@ -11539,22 +11587,26 @@
         <v>1280</v>
       </c>
       <c r="P14" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q14" s="235">
+        <v>594</v>
+      </c>
+      <c r="Q14" s="197">
         <f t="shared" si="0"/>
         <v>0.59375</v>
       </c>
-      <c r="R14" s="235">
+      <c r="R14" s="197">
         <f t="shared" si="0"/>
         <v>0.9375</v>
       </c>
-      <c r="S14" s="235">
+      <c r="S14" s="197">
         <f t="shared" si="0"/>
         <v>1.171875</v>
       </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N15">
         <v>5</v>
       </c>
@@ -11563,19 +11615,23 @@
         <v>1600</v>
       </c>
       <c r="P15" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q15" s="235">
+        <v>594</v>
+      </c>
+      <c r="Q15" s="197">
         <f t="shared" si="0"/>
         <v>0.47499999999999998</v>
       </c>
-      <c r="R15" s="235">
+      <c r="R15" s="197">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="S15" s="235">
+      <c r="S15" s="197">
         <f t="shared" si="0"/>
         <v>0.9375</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>6400</v>
       </c>
     </row>
   </sheetData>
@@ -11588,8 +11644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11618,169 +11674,169 @@
       <c r="D4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="227" t="s">
+      <c r="E4" s="189" t="s">
         <v>561</v>
       </c>
-      <c r="F4" s="227" t="s">
+      <c r="F4" s="189" t="s">
         <v>572</v>
       </c>
-      <c r="G4" s="227" t="s">
+      <c r="G4" s="189" t="s">
         <v>562</v>
       </c>
-      <c r="H4" s="227" t="s">
+      <c r="H4" s="189" t="s">
         <v>565</v>
       </c>
-      <c r="I4" s="227" t="s">
+      <c r="I4" s="189" t="s">
         <v>568</v>
       </c>
-      <c r="J4" s="227" t="s">
+      <c r="J4" s="189" t="s">
+        <v>574</v>
+      </c>
+      <c r="K4" s="189" t="s">
         <v>575</v>
       </c>
-      <c r="K4" s="227" t="s">
-        <v>576</v>
-      </c>
-      <c r="L4" s="227" t="s">
-        <v>578</v>
+      <c r="L4" s="189" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="226" t="s">
+      <c r="B5" s="188" t="s">
         <v>571</v>
       </c>
       <c r="C5" t="s">
+        <v>587</v>
+      </c>
+      <c r="D5" s="188" t="s">
         <v>588</v>
       </c>
-      <c r="D5" s="226" t="s">
+      <c r="E5" s="190">
+        <v>4</v>
+      </c>
+      <c r="F5" s="190">
+        <v>125</v>
+      </c>
+      <c r="G5" s="190" t="s">
+        <v>563</v>
+      </c>
+      <c r="H5" s="190" t="s">
+        <v>563</v>
+      </c>
+      <c r="I5" s="190" t="s">
+        <v>564</v>
+      </c>
+      <c r="J5" s="191"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="188" t="s">
+        <v>557</v>
+      </c>
+      <c r="C6" t="s">
+        <v>587</v>
+      </c>
+      <c r="D6" s="188" t="s">
         <v>589</v>
       </c>
-      <c r="E5" s="228">
-        <v>4</v>
-      </c>
-      <c r="F5" s="228">
-        <v>125</v>
-      </c>
-      <c r="G5" s="228" t="s">
+      <c r="E6" s="190">
+        <v>6</v>
+      </c>
+      <c r="F6" s="190">
+        <v>86</v>
+      </c>
+      <c r="G6" s="190" t="s">
         <v>563</v>
       </c>
-      <c r="H5" s="228" t="s">
+      <c r="H6" s="190" t="s">
+        <v>566</v>
+      </c>
+      <c r="I6" s="190" t="s">
+        <v>569</v>
+      </c>
+      <c r="J6" s="191"/>
+      <c r="K6" s="41"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="188" t="s">
+        <v>586</v>
+      </c>
+      <c r="C7" t="s">
+        <v>587</v>
+      </c>
+      <c r="D7" s="188" t="s">
+        <v>590</v>
+      </c>
+      <c r="E7" s="190">
+        <v>6</v>
+      </c>
+      <c r="F7" s="190">
+        <v>67</v>
+      </c>
+      <c r="G7" s="196" t="s">
         <v>563</v>
       </c>
-      <c r="I5" s="228" t="s">
+      <c r="H7" s="196" t="s">
+        <v>567</v>
+      </c>
+      <c r="I7" s="196" t="s">
+        <v>570</v>
+      </c>
+      <c r="J7" s="191">
+        <v>7960</v>
+      </c>
+      <c r="K7" s="41"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="188" t="s">
+        <v>560</v>
+      </c>
+      <c r="C8" t="s">
+        <v>587</v>
+      </c>
+      <c r="D8" s="188" t="s">
+        <v>591</v>
+      </c>
+      <c r="E8" s="190">
+        <v>6</v>
+      </c>
+      <c r="F8" s="190">
+        <v>86</v>
+      </c>
+      <c r="G8" s="196" t="s">
         <v>564</v>
       </c>
-      <c r="J5" s="229"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="226" t="s">
-        <v>557</v>
-      </c>
-      <c r="C6" t="s">
-        <v>588</v>
-      </c>
-      <c r="D6" s="226" t="s">
-        <v>590</v>
-      </c>
-      <c r="E6" s="228">
+      <c r="H8" s="196" t="s">
+        <v>567</v>
+      </c>
+      <c r="I8" s="196" t="s">
+        <v>570</v>
+      </c>
+      <c r="J8" s="191">
+        <v>11100</v>
+      </c>
+      <c r="K8" s="41"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="188" t="s">
+        <v>573</v>
+      </c>
+      <c r="C9" t="s">
+        <v>587</v>
+      </c>
+      <c r="D9" s="188" t="s">
+        <v>592</v>
+      </c>
+      <c r="E9" s="190">
         <v>6</v>
       </c>
-      <c r="F6" s="228">
-        <v>86</v>
-      </c>
-      <c r="G6" s="228" t="s">
-        <v>563</v>
-      </c>
-      <c r="H6" s="228" t="s">
-        <v>566</v>
-      </c>
-      <c r="I6" s="228" t="s">
-        <v>569</v>
-      </c>
-      <c r="J6" s="229"/>
-      <c r="K6" s="41"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="226" t="s">
-        <v>587</v>
-      </c>
-      <c r="C7" t="s">
-        <v>588</v>
-      </c>
-      <c r="D7" s="226" t="s">
-        <v>591</v>
-      </c>
-      <c r="E7" s="228">
-        <v>6</v>
-      </c>
-      <c r="F7" s="228">
-        <v>67</v>
-      </c>
-      <c r="G7" s="234" t="s">
-        <v>563</v>
-      </c>
-      <c r="H7" s="234" t="s">
+      <c r="F9" s="190">
+        <v>100</v>
+      </c>
+      <c r="G9" s="196" t="s">
+        <v>564</v>
+      </c>
+      <c r="H9" s="196" t="s">
         <v>567</v>
       </c>
-      <c r="I7" s="234" t="s">
-        <v>570</v>
-      </c>
-      <c r="J7" s="229">
-        <v>7960</v>
-      </c>
-      <c r="K7" s="41"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="226" t="s">
-        <v>560</v>
-      </c>
-      <c r="C8" t="s">
-        <v>588</v>
-      </c>
-      <c r="D8" s="226" t="s">
-        <v>592</v>
-      </c>
-      <c r="E8" s="228">
-        <v>6</v>
-      </c>
-      <c r="F8" s="228">
-        <v>86</v>
-      </c>
-      <c r="G8" s="234" t="s">
-        <v>564</v>
-      </c>
-      <c r="H8" s="234" t="s">
-        <v>567</v>
-      </c>
-      <c r="I8" s="234" t="s">
-        <v>570</v>
-      </c>
-      <c r="J8" s="229">
-        <v>11100</v>
-      </c>
-      <c r="K8" s="41"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="226" t="s">
-        <v>573</v>
-      </c>
-      <c r="C9" t="s">
-        <v>588</v>
-      </c>
-      <c r="D9" s="226" t="s">
-        <v>593</v>
-      </c>
-      <c r="E9" s="228">
-        <v>6</v>
-      </c>
-      <c r="F9" s="228">
-        <v>100</v>
-      </c>
-      <c r="G9" s="234" t="s">
-        <v>564</v>
-      </c>
-      <c r="H9" s="234" t="s">
-        <v>567</v>
-      </c>
-      <c r="I9" s="234" t="s">
+      <c r="I9" s="196" t="s">
         <v>570</v>
       </c>
       <c r="J9" s="41"/>
@@ -11792,28 +11848,28 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="226" t="s">
-        <v>574</v>
+      <c r="B10" s="188" t="s">
+        <v>601</v>
       </c>
       <c r="C10" t="s">
-        <v>588</v>
-      </c>
-      <c r="D10" s="226" t="s">
-        <v>594</v>
-      </c>
-      <c r="E10" s="228">
+        <v>587</v>
+      </c>
+      <c r="D10" s="188" t="s">
+        <v>593</v>
+      </c>
+      <c r="E10" s="190">
         <v>6</v>
       </c>
-      <c r="F10" s="228">
+      <c r="F10" s="190">
         <v>125</v>
       </c>
-      <c r="G10" s="234" t="s">
+      <c r="G10" s="196" t="s">
         <v>564</v>
       </c>
-      <c r="H10" s="234" t="s">
+      <c r="H10" s="196" t="s">
         <v>567</v>
       </c>
-      <c r="I10" s="234" t="s">
+      <c r="I10" s="196" t="s">
         <v>570</v>
       </c>
       <c r="J10" s="41"/>
@@ -11821,32 +11877,32 @@
         <v>13596</v>
       </c>
       <c r="L10" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="226" t="s">
-        <v>577</v>
+      <c r="B11" s="188" t="s">
+        <v>576</v>
       </c>
       <c r="C11" t="s">
-        <v>588</v>
-      </c>
-      <c r="D11" s="226" t="s">
-        <v>594</v>
-      </c>
-      <c r="E11" s="228">
+        <v>587</v>
+      </c>
+      <c r="D11" s="188" t="s">
+        <v>593</v>
+      </c>
+      <c r="E11" s="190">
         <v>6</v>
       </c>
-      <c r="F11" s="228">
+      <c r="F11" s="190">
         <v>125</v>
       </c>
-      <c r="G11" s="234" t="s">
+      <c r="G11" s="196" t="s">
         <v>564</v>
       </c>
-      <c r="H11" s="234" t="s">
+      <c r="H11" s="196" t="s">
         <v>567</v>
       </c>
-      <c r="I11" s="234" t="s">
+      <c r="I11" s="196" t="s">
         <v>570</v>
       </c>
       <c r="J11" s="41"/>

</xml_diff>

<commit_message>
[Pipette] Trans current 측정 결과 update
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Review Data_20180203.xlsx
+++ b/Plasma_Gen_Review Data_20180203.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12975" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="시제품_Pulse" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="604">
   <si>
     <t>각 mode 별 Pulse 출력</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2456,10 +2456,6 @@
   </si>
   <si>
     <t>CTX210611-R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Current Probe 설정 AC로 측정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -3471,6 +3467,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3489,63 +3530,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3556,12 +3558,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5147,20 +5143,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>174913</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>464400</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>19497</xdr:rowOff>
+      <xdr:colOff>355450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>96860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="6" name="그림 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5179,8 +5175,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="400050" y="3676651"/>
-          <a:ext cx="7551000" cy="5162996"/>
+          <a:off x="815686" y="1783773"/>
+          <a:ext cx="7107809" cy="4790087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5191,20 +5187,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>235725</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>7126</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>105838</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>195028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>671550</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>140922</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>286375</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>187978</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="7" name="그림 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5223,8 +5219,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8408175" y="3798076"/>
-          <a:ext cx="7551000" cy="5162996"/>
+          <a:off x="746611" y="6672028"/>
+          <a:ext cx="7107809" cy="4772768"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5235,20 +5231,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>33300</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>23776</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>103438</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>22910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>402450</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>157572</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>26800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>15860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="8" name="그림 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5267,8 +5263,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="338100" y="9263026"/>
-          <a:ext cx="7551000" cy="5162996"/>
+          <a:off x="8364211" y="6707728"/>
+          <a:ext cx="7093089" cy="4772768"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5279,20 +5275,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>240450</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>21376</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>110563</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>30034</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>155172</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>291100</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>22984</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPr id="9" name="그림 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5311,8 +5307,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8412900" y="9260626"/>
-          <a:ext cx="7551000" cy="5162996"/>
+          <a:off x="751336" y="11702489"/>
+          <a:ext cx="7107809" cy="4772768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12913</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>206878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>622075</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>199827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8273686" y="11671514"/>
+          <a:ext cx="7086162" cy="4772768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>58138</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>25234</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238675</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>18185</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="그림 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698911" y="16685325"/>
+          <a:ext cx="7107809" cy="4772769"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6308,10 +6392,10 @@
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="222" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="208"/>
+      <c r="C3" s="223"/>
       <c r="D3" s="13">
         <v>128</v>
       </c>
@@ -6330,10 +6414,10 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="209" t="s">
+      <c r="B4" s="224" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="210"/>
+      <c r="C4" s="225"/>
       <c r="D4" s="16">
         <v>16</v>
       </c>
@@ -6353,10 +6437,10 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="209" t="s">
+      <c r="B5" s="224" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="210"/>
+      <c r="C5" s="225"/>
       <c r="D5" s="16">
         <v>48</v>
       </c>
@@ -6378,10 +6462,10 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="209" t="s">
+      <c r="B6" s="224" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="210"/>
+      <c r="C6" s="225"/>
       <c r="D6" s="16" t="s">
         <v>34</v>
       </c>
@@ -6398,10 +6482,10 @@
       <c r="Q6" s="67"/>
     </row>
     <row r="7" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="226" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="212"/>
+      <c r="C7" s="227"/>
       <c r="D7" s="19" t="s">
         <v>37</v>
       </c>
@@ -6470,39 +6554,39 @@
     </row>
     <row r="13" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="220" t="s">
+      <c r="B14" s="218" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="214"/>
-      <c r="D14" s="214" t="s">
+      <c r="C14" s="212"/>
+      <c r="D14" s="212" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="214" t="s">
+      <c r="E14" s="212" t="s">
         <v>236</v>
       </c>
-      <c r="F14" s="215"/>
-      <c r="G14" s="221" t="s">
+      <c r="F14" s="213"/>
+      <c r="G14" s="219" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="222"/>
-      <c r="I14" s="221" t="s">
+      <c r="H14" s="220"/>
+      <c r="I14" s="219" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="222"/>
-      <c r="K14" s="221" t="s">
+      <c r="J14" s="220"/>
+      <c r="K14" s="219" t="s">
         <v>224</v>
       </c>
-      <c r="L14" s="213"/>
+      <c r="L14" s="211"/>
       <c r="M14" s="78"/>
       <c r="N14" s="96"/>
-      <c r="O14" s="221" t="s">
+      <c r="O14" s="219" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="213"/>
-      <c r="Q14" s="213" t="s">
+      <c r="P14" s="211"/>
+      <c r="Q14" s="211" t="s">
         <v>225</v>
       </c>
-      <c r="R14" s="213"/>
+      <c r="R14" s="211"/>
       <c r="S14" s="129"/>
       <c r="T14" s="94"/>
     </row>
@@ -6513,7 +6597,7 @@
       <c r="C15" s="64" t="s">
         <v>251</v>
       </c>
-      <c r="D15" s="223"/>
+      <c r="D15" s="221"/>
       <c r="E15" s="64" t="s">
         <v>320</v>
       </c>
@@ -6573,10 +6657,10 @@
       <c r="D16" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="216" t="s">
+      <c r="E16" s="214" t="s">
         <v>247</v>
       </c>
-      <c r="F16" s="217"/>
+      <c r="F16" s="215"/>
       <c r="G16" s="111"/>
       <c r="H16" s="144"/>
       <c r="I16" s="154"/>
@@ -6823,10 +6907,10 @@
       <c r="D22" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="218" t="s">
+      <c r="E22" s="216" t="s">
         <v>248</v>
       </c>
-      <c r="F22" s="219"/>
+      <c r="F22" s="217"/>
       <c r="G22" s="139"/>
       <c r="H22" s="98"/>
       <c r="I22" s="84"/>
@@ -7070,10 +7154,10 @@
       <c r="D27" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="E27" s="224" t="s">
+      <c r="E27" s="207" t="s">
         <v>260</v>
       </c>
-      <c r="F27" s="225"/>
+      <c r="F27" s="208"/>
       <c r="G27" s="140"/>
       <c r="H27" s="100"/>
       <c r="I27" s="84"/>
@@ -7099,10 +7183,10 @@
       <c r="D28" s="82" t="s">
         <v>259</v>
       </c>
-      <c r="E28" s="224" t="s">
+      <c r="E28" s="207" t="s">
         <v>261</v>
       </c>
-      <c r="F28" s="225"/>
+      <c r="F28" s="208"/>
       <c r="G28" s="140"/>
       <c r="H28" s="100"/>
       <c r="I28" s="84"/>
@@ -7300,10 +7384,10 @@
       <c r="D33" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E33" s="224" t="s">
+      <c r="E33" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F33" s="225"/>
+      <c r="F33" s="208"/>
       <c r="G33" s="140"/>
       <c r="H33" s="100"/>
       <c r="I33" s="84"/>
@@ -7329,10 +7413,10 @@
       <c r="D34" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E34" s="224" t="s">
+      <c r="E34" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="F34" s="225"/>
+      <c r="F34" s="208"/>
       <c r="G34" s="140"/>
       <c r="H34" s="100"/>
       <c r="I34" s="84"/>
@@ -7962,10 +8046,10 @@
       <c r="D46" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E46" s="224" t="s">
+      <c r="E46" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F46" s="225"/>
+      <c r="F46" s="208"/>
       <c r="G46" s="140"/>
       <c r="H46" s="100"/>
       <c r="I46" s="84"/>
@@ -7991,10 +8075,10 @@
       <c r="D47" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="224" t="s">
+      <c r="E47" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="F47" s="225"/>
+      <c r="F47" s="208"/>
       <c r="G47" s="140"/>
       <c r="H47" s="100"/>
       <c r="I47" s="84"/>
@@ -8735,10 +8819,10 @@
       <c r="D62" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E62" s="224" t="s">
+      <c r="E62" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F62" s="225"/>
+      <c r="F62" s="208"/>
       <c r="G62" s="140"/>
       <c r="H62" s="100"/>
       <c r="I62" s="84"/>
@@ -8764,10 +8848,10 @@
       <c r="D63" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E63" s="224" t="s">
+      <c r="E63" s="207" t="s">
         <v>247</v>
       </c>
-      <c r="F63" s="225"/>
+      <c r="F63" s="208"/>
       <c r="G63" s="140"/>
       <c r="H63" s="100"/>
       <c r="I63" s="84"/>
@@ -9378,10 +9462,10 @@
       <c r="D75" s="109" t="s">
         <v>297</v>
       </c>
-      <c r="E75" s="224" t="s">
+      <c r="E75" s="207" t="s">
         <v>316</v>
       </c>
-      <c r="F75" s="225"/>
+      <c r="F75" s="208"/>
       <c r="G75" s="140"/>
       <c r="H75" s="136"/>
       <c r="I75" s="85"/>
@@ -9529,10 +9613,10 @@
       <c r="D78" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E78" s="224" t="s">
+      <c r="E78" s="207" t="s">
         <v>267</v>
       </c>
-      <c r="F78" s="225"/>
+      <c r="F78" s="208"/>
       <c r="G78" s="140"/>
       <c r="H78" s="100"/>
       <c r="I78" s="84"/>
@@ -9558,10 +9642,10 @@
       <c r="D79" s="88" t="s">
         <v>235</v>
       </c>
-      <c r="E79" s="226" t="s">
+      <c r="E79" s="209" t="s">
         <v>247</v>
       </c>
-      <c r="F79" s="227"/>
+      <c r="F79" s="210"/>
       <c r="G79" s="141"/>
       <c r="H79" s="143"/>
       <c r="I79" s="148"/>
@@ -9628,17 +9712,11 @@
   </sheetData>
   <autoFilter ref="B15:AB79"/>
   <mergeCells count="26">
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E16:F16"/>
@@ -9649,11 +9727,17 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="O14:P14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E75:F75"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9718,7 +9802,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="228" t="s">
+      <c r="B4" s="233" t="s">
         <v>332</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -9743,7 +9827,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="229"/>
+      <c r="B5" s="230"/>
       <c r="C5" s="7" t="s">
         <v>211</v>
       </c>
@@ -9763,7 +9847,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="229"/>
+      <c r="B6" s="230"/>
       <c r="C6" s="7" t="s">
         <v>218</v>
       </c>
@@ -9783,7 +9867,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="229" t="s">
+      <c r="B7" s="230" t="s">
         <v>217</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -9805,7 +9889,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="229"/>
+      <c r="B8" s="230"/>
       <c r="C8" s="7" t="s">
         <v>219</v>
       </c>
@@ -9825,7 +9909,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="229" t="s">
+      <c r="B9" s="230" t="s">
         <v>226</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -9845,7 +9929,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="230"/>
+      <c r="B10" s="231"/>
       <c r="C10" s="9" t="s">
         <v>231</v>
       </c>
@@ -9865,7 +9949,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="231" t="s">
+      <c r="B11" s="232" t="s">
         <v>401</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -9887,7 +9971,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="229"/>
+      <c r="B12" s="230"/>
       <c r="C12" s="39" t="s">
         <v>329</v>
       </c>
@@ -9907,7 +9991,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="230"/>
+      <c r="B13" s="231"/>
       <c r="C13" s="45" t="s">
         <v>364</v>
       </c>
@@ -9927,7 +10011,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="231" t="s">
+      <c r="B14" s="232" t="s">
         <v>333</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -9949,7 +10033,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="230"/>
+      <c r="B15" s="231"/>
       <c r="C15" s="45" t="s">
         <v>415</v>
       </c>
@@ -9969,7 +10053,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="234" t="s">
+      <c r="B16" s="236" t="s">
         <v>416</v>
       </c>
       <c r="C16" s="44" t="s">
@@ -9991,7 +10075,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="235"/>
+      <c r="B17" s="237"/>
       <c r="C17" s="119" t="s">
         <v>513</v>
       </c>
@@ -10013,7 +10097,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="235"/>
+      <c r="B18" s="237"/>
       <c r="C18" s="118" t="s">
         <v>522</v>
       </c>
@@ -10033,7 +10117,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="233"/>
+      <c r="B19" s="235"/>
       <c r="C19" s="118" t="s">
         <v>524</v>
       </c>
@@ -10053,7 +10137,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="232" t="s">
+      <c r="B20" s="234" t="s">
         <v>422</v>
       </c>
       <c r="C20" s="39" t="s">
@@ -10075,7 +10159,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="233"/>
+      <c r="B21" s="235"/>
       <c r="C21" s="118" t="s">
         <v>519</v>
       </c>
@@ -10095,7 +10179,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="229" t="s">
+      <c r="B22" s="230" t="s">
         <v>436</v>
       </c>
       <c r="C22" s="39" t="s">
@@ -10117,7 +10201,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="229"/>
+      <c r="B23" s="230"/>
       <c r="C23" s="39" t="s">
         <v>452</v>
       </c>
@@ -10224,7 +10308,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="229" t="s">
+      <c r="B28" s="230" t="s">
         <v>486</v>
       </c>
       <c r="C28" s="39" t="s">
@@ -10249,7 +10333,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="229"/>
+      <c r="B29" s="230"/>
       <c r="C29" s="39" t="s">
         <v>484</v>
       </c>
@@ -10272,7 +10356,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="230"/>
+      <c r="B30" s="231"/>
       <c r="C30" s="45" t="s">
         <v>485</v>
       </c>
@@ -10319,7 +10403,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="237" t="s">
+      <c r="B32" s="229" t="s">
         <v>599</v>
       </c>
       <c r="C32" s="188" t="s">
@@ -10334,7 +10418,7 @@
       <c r="H32" s="41"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="236"/>
+      <c r="B33" s="228"/>
       <c r="C33" s="188" t="s">
         <v>560</v>
       </c>
@@ -10346,7 +10430,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="236"/>
+      <c r="B34" s="228"/>
       <c r="C34" s="188" t="s">
         <v>555</v>
       </c>
@@ -10358,7 +10442,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="236"/>
+      <c r="B35" s="228"/>
       <c r="C35" s="188" t="s">
         <v>557</v>
       </c>
@@ -10370,7 +10454,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="236" t="s">
+      <c r="B36" s="228" t="s">
         <v>579</v>
       </c>
       <c r="C36" s="188" t="s">
@@ -10393,7 +10477,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="236"/>
+      <c r="B37" s="228"/>
       <c r="C37" s="192" t="s">
         <v>583</v>
       </c>
@@ -10421,17 +10505,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10443,7 +10527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="A124" workbookViewId="0">
       <selection activeCell="M150" sqref="M150"/>
     </sheetView>
   </sheetViews>
@@ -11328,7 +11412,7 @@
       </c>
     </row>
     <row r="148" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C148" s="228" t="s">
+      <c r="C148" s="233" t="s">
         <v>401</v>
       </c>
       <c r="D148" s="45" t="s">
@@ -11349,7 +11433,7 @@
       </c>
     </row>
     <row r="149" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C149" s="229"/>
+      <c r="C149" s="230"/>
       <c r="D149" s="7" t="s">
         <v>392</v>
       </c>
@@ -11368,7 +11452,7 @@
       </c>
     </row>
     <row r="150" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C150" s="229"/>
+      <c r="C150" s="230"/>
       <c r="D150" s="7" t="s">
         <v>402</v>
       </c>
@@ -11587,10 +11671,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:U17"/>
+  <dimension ref="B4:U15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11688,10 +11772,10 @@
         <v>1500</v>
       </c>
       <c r="T10" t="s">
+        <v>602</v>
+      </c>
+      <c r="U10" t="s">
         <v>603</v>
-      </c>
-      <c r="U10" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.3">
@@ -11851,11 +11935,6 @@
       <c r="U15">
         <f t="shared" si="2"/>
         <v>800</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Pipette] Transformer Power 검토
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Review Data_20180203.xlsx
+++ b/Plasma_Gen_Review Data_20180203.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Volume" sheetId="11" r:id="rId7"/>
     <sheet name="Current" sheetId="13" r:id="rId8"/>
     <sheet name="Transformer" sheetId="14" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pin-map'!$B$15:$AB$79</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="610">
   <si>
     <t>각 mode 별 Pulse 출력</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2464,6 +2465,30 @@
   </si>
   <si>
     <t>8V current</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ohm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_load</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_load</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3467,6 +3492,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3479,85 +3555,34 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5981,6 +6006,22 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G31"/>
@@ -6392,10 +6433,10 @@
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="222" t="s">
+      <c r="B3" s="207" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="223"/>
+      <c r="C3" s="208"/>
       <c r="D3" s="13">
         <v>128</v>
       </c>
@@ -6414,10 +6455,10 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="224" t="s">
+      <c r="B4" s="209" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="225"/>
+      <c r="C4" s="210"/>
       <c r="D4" s="16">
         <v>16</v>
       </c>
@@ -6437,10 +6478,10 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="224" t="s">
+      <c r="B5" s="209" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="225"/>
+      <c r="C5" s="210"/>
       <c r="D5" s="16">
         <v>48</v>
       </c>
@@ -6462,10 +6503,10 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="224" t="s">
+      <c r="B6" s="209" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="225"/>
+      <c r="C6" s="210"/>
       <c r="D6" s="16" t="s">
         <v>34</v>
       </c>
@@ -6482,10 +6523,10 @@
       <c r="Q6" s="67"/>
     </row>
     <row r="7" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="226" t="s">
+      <c r="B7" s="211" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="227"/>
+      <c r="C7" s="212"/>
       <c r="D7" s="19" t="s">
         <v>37</v>
       </c>
@@ -6554,39 +6595,39 @@
     </row>
     <row r="13" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="218" t="s">
+      <c r="B14" s="220" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="212"/>
-      <c r="D14" s="212" t="s">
+      <c r="C14" s="214"/>
+      <c r="D14" s="214" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="212" t="s">
+      <c r="E14" s="214" t="s">
         <v>236</v>
       </c>
-      <c r="F14" s="213"/>
-      <c r="G14" s="219" t="s">
+      <c r="F14" s="215"/>
+      <c r="G14" s="221" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="220"/>
-      <c r="I14" s="219" t="s">
+      <c r="H14" s="222"/>
+      <c r="I14" s="221" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="220"/>
-      <c r="K14" s="219" t="s">
+      <c r="J14" s="222"/>
+      <c r="K14" s="221" t="s">
         <v>224</v>
       </c>
-      <c r="L14" s="211"/>
+      <c r="L14" s="213"/>
       <c r="M14" s="78"/>
       <c r="N14" s="96"/>
-      <c r="O14" s="219" t="s">
+      <c r="O14" s="221" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="211"/>
-      <c r="Q14" s="211" t="s">
+      <c r="P14" s="213"/>
+      <c r="Q14" s="213" t="s">
         <v>225</v>
       </c>
-      <c r="R14" s="211"/>
+      <c r="R14" s="213"/>
       <c r="S14" s="129"/>
       <c r="T14" s="94"/>
     </row>
@@ -6597,7 +6638,7 @@
       <c r="C15" s="64" t="s">
         <v>251</v>
       </c>
-      <c r="D15" s="221"/>
+      <c r="D15" s="223"/>
       <c r="E15" s="64" t="s">
         <v>320</v>
       </c>
@@ -6657,10 +6698,10 @@
       <c r="D16" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="214" t="s">
+      <c r="E16" s="216" t="s">
         <v>247</v>
       </c>
-      <c r="F16" s="215"/>
+      <c r="F16" s="217"/>
       <c r="G16" s="111"/>
       <c r="H16" s="144"/>
       <c r="I16" s="154"/>
@@ -6907,10 +6948,10 @@
       <c r="D22" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="216" t="s">
+      <c r="E22" s="218" t="s">
         <v>248</v>
       </c>
-      <c r="F22" s="217"/>
+      <c r="F22" s="219"/>
       <c r="G22" s="139"/>
       <c r="H22" s="98"/>
       <c r="I22" s="84"/>
@@ -7154,10 +7195,10 @@
       <c r="D27" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="E27" s="207" t="s">
+      <c r="E27" s="224" t="s">
         <v>260</v>
       </c>
-      <c r="F27" s="208"/>
+      <c r="F27" s="225"/>
       <c r="G27" s="140"/>
       <c r="H27" s="100"/>
       <c r="I27" s="84"/>
@@ -7183,10 +7224,10 @@
       <c r="D28" s="82" t="s">
         <v>259</v>
       </c>
-      <c r="E28" s="207" t="s">
+      <c r="E28" s="224" t="s">
         <v>261</v>
       </c>
-      <c r="F28" s="208"/>
+      <c r="F28" s="225"/>
       <c r="G28" s="140"/>
       <c r="H28" s="100"/>
       <c r="I28" s="84"/>
@@ -7384,10 +7425,10 @@
       <c r="D33" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E33" s="207" t="s">
+      <c r="E33" s="224" t="s">
         <v>267</v>
       </c>
-      <c r="F33" s="208"/>
+      <c r="F33" s="225"/>
       <c r="G33" s="140"/>
       <c r="H33" s="100"/>
       <c r="I33" s="84"/>
@@ -7413,10 +7454,10 @@
       <c r="D34" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E34" s="207" t="s">
+      <c r="E34" s="224" t="s">
         <v>247</v>
       </c>
-      <c r="F34" s="208"/>
+      <c r="F34" s="225"/>
       <c r="G34" s="140"/>
       <c r="H34" s="100"/>
       <c r="I34" s="84"/>
@@ -8046,10 +8087,10 @@
       <c r="D46" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E46" s="207" t="s">
+      <c r="E46" s="224" t="s">
         <v>267</v>
       </c>
-      <c r="F46" s="208"/>
+      <c r="F46" s="225"/>
       <c r="G46" s="140"/>
       <c r="H46" s="100"/>
       <c r="I46" s="84"/>
@@ -8075,10 +8116,10 @@
       <c r="D47" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E47" s="207" t="s">
+      <c r="E47" s="224" t="s">
         <v>247</v>
       </c>
-      <c r="F47" s="208"/>
+      <c r="F47" s="225"/>
       <c r="G47" s="140"/>
       <c r="H47" s="100"/>
       <c r="I47" s="84"/>
@@ -8819,10 +8860,10 @@
       <c r="D62" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E62" s="207" t="s">
+      <c r="E62" s="224" t="s">
         <v>267</v>
       </c>
-      <c r="F62" s="208"/>
+      <c r="F62" s="225"/>
       <c r="G62" s="140"/>
       <c r="H62" s="100"/>
       <c r="I62" s="84"/>
@@ -8848,10 +8889,10 @@
       <c r="D63" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="E63" s="207" t="s">
+      <c r="E63" s="224" t="s">
         <v>247</v>
       </c>
-      <c r="F63" s="208"/>
+      <c r="F63" s="225"/>
       <c r="G63" s="140"/>
       <c r="H63" s="100"/>
       <c r="I63" s="84"/>
@@ -9462,10 +9503,10 @@
       <c r="D75" s="109" t="s">
         <v>297</v>
       </c>
-      <c r="E75" s="207" t="s">
+      <c r="E75" s="224" t="s">
         <v>316</v>
       </c>
-      <c r="F75" s="208"/>
+      <c r="F75" s="225"/>
       <c r="G75" s="140"/>
       <c r="H75" s="136"/>
       <c r="I75" s="85"/>
@@ -9613,10 +9654,10 @@
       <c r="D78" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="E78" s="207" t="s">
+      <c r="E78" s="224" t="s">
         <v>267</v>
       </c>
-      <c r="F78" s="208"/>
+      <c r="F78" s="225"/>
       <c r="G78" s="140"/>
       <c r="H78" s="100"/>
       <c r="I78" s="84"/>
@@ -9642,10 +9683,10 @@
       <c r="D79" s="88" t="s">
         <v>235</v>
       </c>
-      <c r="E79" s="209" t="s">
+      <c r="E79" s="226" t="s">
         <v>247</v>
       </c>
-      <c r="F79" s="210"/>
+      <c r="F79" s="227"/>
       <c r="G79" s="141"/>
       <c r="H79" s="143"/>
       <c r="I79" s="148"/>
@@ -9712,11 +9753,17 @@
   </sheetData>
   <autoFilter ref="B15:AB79"/>
   <mergeCells count="26">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E46:F46"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E16:F16"/>
@@ -9727,17 +9774,11 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="O14:P14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9802,7 +9843,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="233" t="s">
+      <c r="B4" s="228" t="s">
         <v>332</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -9827,7 +9868,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="230"/>
+      <c r="B5" s="229"/>
       <c r="C5" s="7" t="s">
         <v>211</v>
       </c>
@@ -9847,7 +9888,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="230"/>
+      <c r="B6" s="229"/>
       <c r="C6" s="7" t="s">
         <v>218</v>
       </c>
@@ -9867,7 +9908,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="230" t="s">
+      <c r="B7" s="229" t="s">
         <v>217</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -9889,7 +9930,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="230"/>
+      <c r="B8" s="229"/>
       <c r="C8" s="7" t="s">
         <v>219</v>
       </c>
@@ -9909,7 +9950,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="230" t="s">
+      <c r="B9" s="229" t="s">
         <v>226</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -9929,7 +9970,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="231"/>
+      <c r="B10" s="230"/>
       <c r="C10" s="9" t="s">
         <v>231</v>
       </c>
@@ -9949,7 +9990,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="232" t="s">
+      <c r="B11" s="231" t="s">
         <v>401</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -9971,7 +10012,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="230"/>
+      <c r="B12" s="229"/>
       <c r="C12" s="39" t="s">
         <v>329</v>
       </c>
@@ -9991,7 +10032,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="231"/>
+      <c r="B13" s="230"/>
       <c r="C13" s="45" t="s">
         <v>364</v>
       </c>
@@ -10011,7 +10052,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="232" t="s">
+      <c r="B14" s="231" t="s">
         <v>333</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -10033,7 +10074,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="231"/>
+      <c r="B15" s="230"/>
       <c r="C15" s="45" t="s">
         <v>415</v>
       </c>
@@ -10053,7 +10094,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="236" t="s">
+      <c r="B16" s="234" t="s">
         <v>416</v>
       </c>
       <c r="C16" s="44" t="s">
@@ -10075,7 +10116,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="237"/>
+      <c r="B17" s="235"/>
       <c r="C17" s="119" t="s">
         <v>513</v>
       </c>
@@ -10097,7 +10138,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="237"/>
+      <c r="B18" s="235"/>
       <c r="C18" s="118" t="s">
         <v>522</v>
       </c>
@@ -10117,7 +10158,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="235"/>
+      <c r="B19" s="233"/>
       <c r="C19" s="118" t="s">
         <v>524</v>
       </c>
@@ -10137,7 +10178,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="234" t="s">
+      <c r="B20" s="232" t="s">
         <v>422</v>
       </c>
       <c r="C20" s="39" t="s">
@@ -10159,7 +10200,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="235"/>
+      <c r="B21" s="233"/>
       <c r="C21" s="118" t="s">
         <v>519</v>
       </c>
@@ -10179,7 +10220,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="230" t="s">
+      <c r="B22" s="229" t="s">
         <v>436</v>
       </c>
       <c r="C22" s="39" t="s">
@@ -10201,7 +10242,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="230"/>
+      <c r="B23" s="229"/>
       <c r="C23" s="39" t="s">
         <v>452</v>
       </c>
@@ -10308,7 +10349,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="230" t="s">
+      <c r="B28" s="229" t="s">
         <v>486</v>
       </c>
       <c r="C28" s="39" t="s">
@@ -10333,7 +10374,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="230"/>
+      <c r="B29" s="229"/>
       <c r="C29" s="39" t="s">
         <v>484</v>
       </c>
@@ -10356,7 +10397,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="231"/>
+      <c r="B30" s="230"/>
       <c r="C30" s="45" t="s">
         <v>485</v>
       </c>
@@ -10403,7 +10444,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="229" t="s">
+      <c r="B32" s="237" t="s">
         <v>599</v>
       </c>
       <c r="C32" s="188" t="s">
@@ -10418,7 +10459,7 @@
       <c r="H32" s="41"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="228"/>
+      <c r="B33" s="236"/>
       <c r="C33" s="188" t="s">
         <v>560</v>
       </c>
@@ -10430,7 +10471,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="228"/>
+      <c r="B34" s="236"/>
       <c r="C34" s="188" t="s">
         <v>555</v>
       </c>
@@ -10442,7 +10483,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="228"/>
+      <c r="B35" s="236"/>
       <c r="C35" s="188" t="s">
         <v>557</v>
       </c>
@@ -10454,7 +10495,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="228" t="s">
+      <c r="B36" s="236" t="s">
         <v>579</v>
       </c>
       <c r="C36" s="188" t="s">
@@ -10477,7 +10518,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="228"/>
+      <c r="B37" s="236"/>
       <c r="C37" s="192" t="s">
         <v>583</v>
       </c>
@@ -10505,17 +10546,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11412,7 +11453,7 @@
       </c>
     </row>
     <row r="148" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C148" s="233" t="s">
+      <c r="C148" s="228" t="s">
         <v>401</v>
       </c>
       <c r="D148" s="45" t="s">
@@ -11433,7 +11474,7 @@
       </c>
     </row>
     <row r="149" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C149" s="230"/>
+      <c r="C149" s="229"/>
       <c r="D149" s="7" t="s">
         <v>392</v>
       </c>
@@ -11452,7 +11493,7 @@
       </c>
     </row>
     <row r="150" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C150" s="230"/>
+      <c r="C150" s="229"/>
       <c r="D150" s="7" t="s">
         <v>402</v>
       </c>
@@ -11671,10 +11712,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:U15"/>
+  <dimension ref="B4:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11935,6 +11976,40 @@
       <c r="U15">
         <f t="shared" si="2"/>
         <v>800</v>
+      </c>
+    </row>
+    <row r="20" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>607</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="21" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>608</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="22" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>609</v>
+      </c>
+      <c r="O22">
+        <f>O20/O21</f>
+        <v>2</v>
+      </c>
+      <c r="P22" t="s">
+        <v>606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>